<commit_message>
Las funciones de dano funcionan correctamente con marco de un nivel
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0_error.xlsx
+++ b/pruebas_excel/marco3Ddam0_error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral_error\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AC16B4-EC36-443E-987C-424EDEE7ADD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7D7AF3-D14F-4627-A4E9-461F4AA1766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="5115" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
   <si>
     <t>Marco 3D</t>
   </si>
@@ -13604,7 +13604,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13624,7 +13624,7 @@
         <v>5000</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13669,15 +13669,61 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
@@ -74618,22 +74664,22 @@
       </c>
       <c r="N8">
         <f>'prop geom'!B9</f>
-        <v>0</v>
+        <v>11721.3</v>
       </c>
       <c r="O8">
         <v>4000</v>
       </c>
       <c r="P8">
         <f>N8*O8</f>
-        <v>0</v>
+        <v>46885200</v>
       </c>
       <c r="Q8" s="2">
         <f>P8*M8</f>
-        <v>0</v>
+        <v>0.11252448</v>
       </c>
       <c r="R8" s="2">
         <f>Q8/2</f>
-        <v>0</v>
+        <v>5.6262239999999998E-2</v>
       </c>
       <c r="S8" t="s">
         <v>62</v>
@@ -74682,22 +74728,22 @@
       </c>
       <c r="N9">
         <f>'prop geom'!B11</f>
-        <v>0</v>
+        <v>11721.3</v>
       </c>
       <c r="O9">
         <v>6000</v>
       </c>
       <c r="P9">
         <f>N9*O9</f>
-        <v>0</v>
+        <v>70327800</v>
       </c>
       <c r="Q9" s="2">
         <f>P9*M9</f>
-        <v>0</v>
+        <v>0.16878672</v>
       </c>
       <c r="R9" s="2">
         <f>Q9/2</f>
-        <v>0</v>
+        <v>8.4393360000000001E-2</v>
       </c>
       <c r="S9" t="s">
         <v>64</v>
@@ -74741,7 +74787,7 @@
       </c>
       <c r="N12" s="2">
         <f>R8</f>
-        <v>0</v>
+        <v>5.6262239999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -74753,7 +74799,7 @@
       </c>
       <c r="N13" s="2">
         <f>R8+R9+R10</f>
-        <v>0</v>
+        <v>0.14065559999999999</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -74762,7 +74808,7 @@
       </c>
       <c r="N14" s="2">
         <f>R8</f>
-        <v>0</v>
+        <v>5.6262239999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -74771,7 +74817,7 @@
       </c>
       <c r="N15" s="2">
         <f>N13</f>
-        <v>0</v>
+        <v>0.14065559999999999</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -74804,7 +74850,7 @@
       </c>
       <c r="N16" s="2">
         <f>R8</f>
-        <v>0</v>
+        <v>5.6262239999999998E-2</v>
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
@@ -74837,7 +74883,7 @@
       </c>
       <c r="N17" s="2">
         <f>N15</f>
-        <v>0</v>
+        <v>0.14065559999999999</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
@@ -74870,7 +74916,7 @@
       </c>
       <c r="N18" s="2">
         <f>R8</f>
-        <v>0</v>
+        <v>5.6262239999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
@@ -74903,7 +74949,7 @@
       </c>
       <c r="N19" s="2">
         <f>N17</f>
-        <v>0</v>
+        <v>0.14065559999999999</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
@@ -75069,10 +75115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75127,7 +75173,130 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -75136,10 +75305,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D051BC6-55A0-4B3B-BADC-15C4CA1EE579}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75157,7 +75326,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -75180,6 +75349,105 @@
       </c>
       <c r="C3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -75192,7 +75460,7 @@
   <dimension ref="A1:Q182"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N3"/>
+      <selection sqref="A1:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75340,148 +75608,400 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="A4" s="12">
+        <v>4</v>
+      </c>
+      <c r="B4" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C4" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D4" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E4" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F4" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G4" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="12">
+        <v>300</v>
+      </c>
+      <c r="K4" s="12">
+        <v>300</v>
+      </c>
+      <c r="L4" s="12">
+        <v>13</v>
+      </c>
+      <c r="M4" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C5" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D5" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E5" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F5" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G5" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="12">
+        <v>300</v>
+      </c>
+      <c r="K5" s="12">
+        <v>300</v>
+      </c>
+      <c r="L5" s="12">
+        <v>13</v>
+      </c>
+      <c r="M5" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="A6" s="12">
+        <v>6</v>
+      </c>
+      <c r="B6" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C6" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D6" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E6" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F6" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G6" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="12">
+        <v>300</v>
+      </c>
+      <c r="K6" s="12">
+        <v>300</v>
+      </c>
+      <c r="L6" s="12">
+        <v>13</v>
+      </c>
+      <c r="M6" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="A7" s="12">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D7" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E7" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F7" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G7" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="12">
+        <v>300</v>
+      </c>
+      <c r="K7" s="12">
+        <v>300</v>
+      </c>
+      <c r="L7" s="12">
+        <v>13</v>
+      </c>
+      <c r="M7" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="A8" s="12">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C8" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D8" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E8" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F8" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G8" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="12">
+        <v>300</v>
+      </c>
+      <c r="K8" s="12">
+        <v>300</v>
+      </c>
+      <c r="L8" s="12">
+        <v>13</v>
+      </c>
+      <c r="M8" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="A9" s="12">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C9" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D9" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E9" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F9" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G9" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="12">
+        <v>300</v>
+      </c>
+      <c r="K9" s="12">
+        <v>300</v>
+      </c>
+      <c r="L9" s="12">
+        <v>13</v>
+      </c>
+      <c r="M9" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N9" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="A10" s="12">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C10" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D10" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E10" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F10" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G10" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="12">
+        <v>300</v>
+      </c>
+      <c r="K10" s="12">
+        <v>300</v>
+      </c>
+      <c r="L10" s="12">
+        <v>13</v>
+      </c>
+      <c r="M10" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="A11" s="12">
+        <v>11</v>
+      </c>
+      <c r="B11" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C11" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D11" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E11" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F11" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G11" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="12">
+        <v>300</v>
+      </c>
+      <c r="K11" s="12">
+        <v>300</v>
+      </c>
+      <c r="L11" s="12">
+        <v>13</v>
+      </c>
+      <c r="M11" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N11" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="A12" s="12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12">
+        <v>11721.3</v>
+      </c>
+      <c r="C12" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="D12" s="12">
+        <v>120931398.7</v>
+      </c>
+      <c r="E12" s="12">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F12" s="12">
+        <v>199947.98</v>
+      </c>
+      <c r="G12" s="12">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="12">
+        <v>300</v>
+      </c>
+      <c r="K12" s="12">
+        <v>300</v>
+      </c>
+      <c r="L12" s="12">
+        <v>13</v>
+      </c>
+      <c r="M12" s="12">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -78180,14 +78700,14 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -78205,6 +78725,75 @@
         <v>1</v>
       </c>
       <c r="G1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
     </row>

</xml_diff>